<commit_message>
small changes to run.py
</commit_message>
<xml_diff>
--- a/cluster_experiments/data/cluster_experiment_details.xlsx
+++ b/cluster_experiments/data/cluster_experiment_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\OneDrive\Documents\GitHub\new\cluster_experiments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD8C12A-67A7-482E-89AF-62722CAF66AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F838DE8-4193-4FF6-BD82-EDF2B96907D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>